<commit_message>
chore: Update readme and config src code
</commit_message>
<xml_diff>
--- a/src/problem-1/data/DSSV.xlsx
+++ b/src/problem-1/data/DSSV.xlsx
@@ -1,32 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final-term-problem-from-multimedia\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIANGDAY\CAU TRUC DU LIEU VA GIAI THUAT\D22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0061E880-EB53-4794-B14D-08B0B68FBEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1206,7 +1194,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1260,10 +1248,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1602,7 +1590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
@@ -1612,14 +1600,14 @@
       <selection pane="bottomRight" activeCell="G145" sqref="G145"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.75" customWidth="1"/>
+    <col min="2" max="2" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1639,7 +1627,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1657,10 +1645,10 @@
       </c>
       <c r="F2" s="1">
         <f ca="1">CEILING(RAND()*10, 1)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1678,10 +1666,10 @@
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F66" ca="1" si="0">CEILING(RAND()*10, 1)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1699,10 +1687,10 @@
       </c>
       <c r="F4" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1720,10 +1708,10 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1741,10 +1729,10 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1762,10 +1750,10 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1783,10 +1771,10 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1804,10 +1792,10 @@
       </c>
       <c r="F9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1825,10 +1813,10 @@
       </c>
       <c r="F10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1846,10 +1834,10 @@
       </c>
       <c r="F11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1867,10 +1855,10 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1888,10 +1876,10 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1909,10 +1897,10 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1930,10 +1918,10 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1951,10 +1939,10 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1975,7 +1963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1993,10 +1981,10 @@
       </c>
       <c r="F18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2014,10 +2002,10 @@
       </c>
       <c r="F19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2035,10 +2023,10 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2056,10 +2044,10 @@
       </c>
       <c r="F21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2077,10 +2065,10 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2098,10 +2086,10 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2119,10 +2107,10 @@
       </c>
       <c r="F24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2140,10 +2128,10 @@
       </c>
       <c r="F25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2161,10 +2149,10 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2182,10 +2170,10 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2203,10 +2191,10 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2224,10 +2212,10 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2245,10 +2233,10 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2266,10 +2254,10 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2287,10 +2275,10 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2308,10 +2296,10 @@
       </c>
       <c r="F33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2329,10 +2317,10 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2350,10 +2338,10 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2371,10 +2359,10 @@
       </c>
       <c r="F36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2395,7 +2383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2413,10 +2401,10 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2437,7 +2425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2455,10 +2443,10 @@
       </c>
       <c r="F40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2476,10 +2464,10 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2497,10 +2485,10 @@
       </c>
       <c r="F42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2518,10 +2506,10 @@
       </c>
       <c r="F43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2539,10 +2527,10 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2560,10 +2548,10 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2581,10 +2569,10 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2602,10 +2590,10 @@
       </c>
       <c r="F47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2623,10 +2611,10 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2644,10 +2632,10 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2665,10 +2653,10 @@
       </c>
       <c r="F50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2686,10 +2674,10 @@
       </c>
       <c r="F51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2707,10 +2695,10 @@
       </c>
       <c r="F52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2728,10 +2716,10 @@
       </c>
       <c r="F53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2749,10 +2737,10 @@
       </c>
       <c r="F54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2770,10 +2758,10 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2791,10 +2779,10 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2812,10 +2800,10 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2836,7 +2824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2854,10 +2842,10 @@
       </c>
       <c r="F59" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2875,10 +2863,10 @@
       </c>
       <c r="F60" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2896,10 +2884,10 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2917,10 +2905,10 @@
       </c>
       <c r="F62" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2938,10 +2926,10 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2959,10 +2947,10 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2980,10 +2968,10 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3001,10 +2989,10 @@
       </c>
       <c r="F66" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3022,10 +3010,10 @@
       </c>
       <c r="F67" s="1">
         <f t="shared" ref="F67:F130" ca="1" si="1">CEILING(RAND()*10, 1)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3046,7 +3034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3064,10 +3052,10 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3085,10 +3073,10 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3106,10 +3094,10 @@
       </c>
       <c r="F71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3127,10 +3115,10 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3148,10 +3136,10 @@
       </c>
       <c r="F73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3169,10 +3157,10 @@
       </c>
       <c r="F74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3190,10 +3178,10 @@
       </c>
       <c r="F75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3211,10 +3199,10 @@
       </c>
       <c r="F76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3232,10 +3220,10 @@
       </c>
       <c r="F77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3253,10 +3241,10 @@
       </c>
       <c r="F78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3274,10 +3262,10 @@
       </c>
       <c r="F79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3295,10 +3283,10 @@
       </c>
       <c r="F80" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3316,10 +3304,10 @@
       </c>
       <c r="F81" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3337,10 +3325,10 @@
       </c>
       <c r="F82" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3358,10 +3346,10 @@
       </c>
       <c r="F83" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3379,10 +3367,10 @@
       </c>
       <c r="F84" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3400,10 +3388,10 @@
       </c>
       <c r="F85" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3421,10 +3409,10 @@
       </c>
       <c r="F86" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3442,10 +3430,10 @@
       </c>
       <c r="F87" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3463,10 +3451,10 @@
       </c>
       <c r="F88" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3484,10 +3472,10 @@
       </c>
       <c r="F89" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3508,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3526,10 +3514,10 @@
       </c>
       <c r="F91" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3547,10 +3535,10 @@
       </c>
       <c r="F92" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3568,10 +3556,10 @@
       </c>
       <c r="F93" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3589,10 +3577,10 @@
       </c>
       <c r="F94" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -3610,10 +3598,10 @@
       </c>
       <c r="F95" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -3631,10 +3619,10 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -3652,10 +3640,10 @@
       </c>
       <c r="F97" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -3673,10 +3661,10 @@
       </c>
       <c r="F98" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -3694,10 +3682,10 @@
       </c>
       <c r="F99" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -3715,10 +3703,10 @@
       </c>
       <c r="F100" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -3736,10 +3724,10 @@
       </c>
       <c r="F101" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -3757,10 +3745,10 @@
       </c>
       <c r="F102" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -3778,10 +3766,10 @@
       </c>
       <c r="F103" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -3799,10 +3787,10 @@
       </c>
       <c r="F104" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -3820,10 +3808,10 @@
       </c>
       <c r="F105" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -3841,10 +3829,10 @@
       </c>
       <c r="F106" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -3862,10 +3850,10 @@
       </c>
       <c r="F107" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -3883,10 +3871,10 @@
       </c>
       <c r="F108" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -3904,10 +3892,10 @@
       </c>
       <c r="F109" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -3925,10 +3913,10 @@
       </c>
       <c r="F110" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -3946,10 +3934,10 @@
       </c>
       <c r="F111" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -3967,10 +3955,10 @@
       </c>
       <c r="F112" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -3988,10 +3976,10 @@
       </c>
       <c r="F113" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4009,10 +3997,10 @@
       </c>
       <c r="F114" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4030,10 +4018,10 @@
       </c>
       <c r="F115" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4051,10 +4039,10 @@
       </c>
       <c r="F116" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4072,10 +4060,10 @@
       </c>
       <c r="F117" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4096,7 +4084,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4114,10 +4102,10 @@
       </c>
       <c r="F119" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4135,10 +4123,10 @@
       </c>
       <c r="F120" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4156,10 +4144,10 @@
       </c>
       <c r="F121" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4177,10 +4165,10 @@
       </c>
       <c r="F122" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4198,10 +4186,10 @@
       </c>
       <c r="F123" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4219,10 +4207,10 @@
       </c>
       <c r="F124" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4240,10 +4228,10 @@
       </c>
       <c r="F125" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4261,10 +4249,10 @@
       </c>
       <c r="F126" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4282,10 +4270,10 @@
       </c>
       <c r="F127" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4303,10 +4291,10 @@
       </c>
       <c r="F128" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4324,10 +4312,10 @@
       </c>
       <c r="F129" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4348,7 +4336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4369,7 +4357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4387,10 +4375,10 @@
       </c>
       <c r="F132" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4408,10 +4396,10 @@
       </c>
       <c r="F133" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4429,10 +4417,10 @@
       </c>
       <c r="F134" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4450,10 +4438,10 @@
       </c>
       <c r="F135" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4474,7 +4462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4492,10 +4480,10 @@
       </c>
       <c r="F137" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4513,10 +4501,10 @@
       </c>
       <c r="F138" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4534,10 +4522,10 @@
       </c>
       <c r="F139" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4555,10 +4543,10 @@
       </c>
       <c r="F140" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4579,7 +4567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4597,10 +4585,10 @@
       </c>
       <c r="F142" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4618,10 +4606,10 @@
       </c>
       <c r="F143" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4639,10 +4627,10 @@
       </c>
       <c r="F144" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4660,10 +4648,10 @@
       </c>
       <c r="F145" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4681,7 +4669,7 @@
       </c>
       <c r="F146" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>